<commit_message>
msg.com Elastic Search and Home page Test update AND Rockettes.com Locators update
</commit_message>
<xml_diff>
--- a/MSG/RockettesAutomatedTesting/data/Rockettes Test Cases.xlsx
+++ b/MSG/RockettesAutomatedTesting/data/Rockettes Test Cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="920" windowWidth="51200" windowHeight="25480" tabRatio="967"/>
+    <workbookView xWindow="0" yWindow="920" windowWidth="51200" windowHeight="25480" tabRatio="967" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -1106,9 +1106,6 @@
     <t>.//*[@id='wrap']/header[3]/div/h1</t>
   </si>
   <si>
-    <t>.//*[@id='wrap']/header[2]/div/h1</t>
-  </si>
-  <si>
     <t>.//*[@id='main']/header/div/h1</t>
   </si>
   <si>
@@ -1125,6 +1122,9 @@
   </si>
   <si>
     <t>//*[@id="select2-showFinder-container"]</t>
+  </si>
+  <si>
+    <t>.//*[@id='primary']/div/div[2]/div[1]/h2</t>
   </si>
 </sst>
 </file>
@@ -2178,8 +2178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5945,8 +5945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C126"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6122,7 +6122,7 @@
         <v>337</v>
       </c>
       <c r="C21" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -6130,7 +6130,7 @@
         <v>338</v>
       </c>
       <c r="C22" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -6279,7 +6279,7 @@
         <v>350</v>
       </c>
       <c r="C41" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -6395,7 +6395,7 @@
         <v>185</v>
       </c>
       <c r="C56" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -6779,7 +6779,7 @@
         <v>282</v>
       </c>
       <c r="B105" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -6802,7 +6802,7 @@
         <v>288</v>
       </c>
       <c r="C108" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -6865,7 +6865,7 @@
         <v>292</v>
       </c>
       <c r="C116" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="16" x14ac:dyDescent="0.2">

</xml_diff>